<commit_message>
"TestResultExcelFilePath" parameter is removed from NI Payroll class- Data provider method
</commit_message>
<xml_diff>
--- a/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Suite 4WeeklyCatA201819.xlsx
+++ b/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Suite 4WeeklyCatA201819.xlsx
@@ -1,28 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\XCDHR\git\XCDHR_Payroll\Salesforce_Core_Framework\src\main\java\com\test\xcdhr\Salesforce_Core_Framework1\salesforce_XLS_Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="390" yWindow="30" windowWidth="14340" windowHeight="4515" activeTab="2"/>
+    <workbookView activeTab="2" windowHeight="4515" windowWidth="14340" xWindow="390" yWindow="30"/>
   </bookViews>
   <sheets>
-    <sheet name="first" sheetId="1" r:id="rId1"/>
-    <sheet name="NI4WeeklyCat_A" sheetId="2" r:id="rId2"/>
-    <sheet name="ProcessPayrollForNIWeekly" sheetId="4" r:id="rId3"/>
-    <sheet name="TestReports" sheetId="5" r:id="rId4"/>
+    <sheet name="first" r:id="rId1" sheetId="1"/>
+    <sheet name="NI4WeeklyCat_A" r:id="rId2" sheetId="2"/>
+    <sheet name="ProcessPayrollForNIWeekly" r:id="rId3" sheetId="4"/>
+    <sheet name="TestReports" r:id="rId4" sheetId="5"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="62">
   <si>
     <t>TC</t>
   </si>
@@ -214,6 +214,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -261,46 +262,46 @@
     </border>
   </borders>
   <cellStyleXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="13">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="2">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="2"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="2"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -317,10 +318,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -355,7 +356,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -407,7 +408,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -512,7 +513,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -521,13 +522,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -537,7 +538,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -546,7 +547,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -555,7 +556,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -565,12 +566,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -601,7 +602,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -620,7 +621,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -632,7 +633,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -641,10 +642,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="48.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="30.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="33.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="48.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="30.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="33.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.44140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -675,7 +676,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="3" s="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -689,7 +690,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="4" s="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>22</v>
       </c>
@@ -703,7 +704,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="45" r="5" s="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>18</v>
       </c>
@@ -731,7 +732,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="30" r="7" s="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>13</v>
       </c>
@@ -745,7 +746,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row ht="75" r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -760,13 +761,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -775,12 +776,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="28.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18.42578125" style="4" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="39.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="28.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="4" width="18.42578125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -960,16 +961,16 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="C2:C10" numberStoredAsText="1"/>
+    <ignoredError numberStoredAsText="1" sqref="C2:C10"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
@@ -978,19 +979,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="51.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="41.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.42578125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="38.5703125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="47.42578125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="11.5703125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="51.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="41.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="22.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="38.5703125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="47.42578125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="7" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="27.6" r="1" s="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>28</v>
       </c>
@@ -1028,7 +1029,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="9" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="37.5" r="2" s="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>50</v>
       </c>
@@ -1326,24 +1327,24 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
-    <hyperlink ref="E3" r:id="rId2" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
-    <hyperlink ref="E4" r:id="rId3" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
-    <hyperlink ref="E5" r:id="rId4" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
-    <hyperlink ref="E6" r:id="rId5" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
-    <hyperlink ref="E7" r:id="rId6" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
-    <hyperlink ref="E8" r:id="rId7" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
-    <hyperlink ref="E9" r:id="rId8" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
-    <hyperlink ref="E10" r:id="rId9" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
-    <hyperlink ref="A2:A10" r:id="rId10" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId1" ref="E2"/>
+    <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId2" ref="E3"/>
+    <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId3" ref="E4"/>
+    <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId4" ref="E5"/>
+    <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId5" ref="E6"/>
+    <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId6" ref="E7"/>
+    <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId7" ref="E8"/>
+    <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId8" ref="E9"/>
+    <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId9" ref="E10"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId10" ref="A2:A10"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId11"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId11" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
@@ -1352,19 +1353,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="35.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="24.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="23.28515625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="42.42578125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.42578125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14.5703125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="26.28515625" style="5" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="50.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="35.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="24.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="23.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="42.42578125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="5" width="26.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="7" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="27.6" r="1" s="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>28</v>
       </c>
@@ -1405,7 +1406,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="9" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="42.75" r="2" s="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>50</v>
       </c>
@@ -1442,10 +1443,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
-    <hyperlink ref="A2" r:id="rId2" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId1" ref="E2"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId2" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId3" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>